<commit_message>
Added CNN & Random Forest results for Breguet Range
</commit_message>
<xml_diff>
--- a/Results/Breguets_Range/CNN_Confidence_score.xlsx
+++ b/Results/Breguets_Range/CNN_Confidence_score.xlsx
@@ -460,33 +460,33 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.7328145248342572</v>
+        <v>0.1839054330529666</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.6244099140167236</v>
+        <v>0.2158649861812592</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1084046108175336</v>
+        <v>0.03195955312829257</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9021976183069313</v>
+        <v>0.9690302269779759</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.059146417835831</v>
+        <v>0.3009774948852012</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.9171101450920105</v>
+        <v>0.2567024827003479</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1420362727438209</v>
+        <v>0.0442750121848533</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8756289304169219</v>
+        <v>0.9576021530073574</v>
       </c>
     </row>
     <row r="4">
@@ -494,101 +494,101 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.010196633885595</v>
+        <v>0.106615139804501</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.7893999814987183</v>
+        <v>0.1699984669685364</v>
       </c>
       <c r="D4" t="n">
-        <v>0.220796652386877</v>
+        <v>0.06338332716403534</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8191372396416883</v>
+        <v>0.9403946577448473</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>1.910473808478493</v>
+        <v>0.09297567629006591</v>
       </c>
       <c r="C5" t="n">
-        <v>1.682307720184326</v>
+        <v>0.1655720621347427</v>
       </c>
       <c r="D5" t="n">
-        <v>0.228166088294167</v>
+        <v>0.07259638584467683</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8142221231567524</v>
+        <v>0.9323171448246987</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.4962239024081158</v>
+        <v>0.238463287110707</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.2552357614040375</v>
+        <v>0.3150076270103455</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2409881410040783</v>
+        <v>0.07654433989963849</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8058094730791739</v>
+        <v>0.9288981075254418</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.9775634445854378</v>
+        <v>0.2498295067060696</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.7171948552131653</v>
+        <v>0.3265554904937744</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2603685893722725</v>
+        <v>0.07672598378770479</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7934186938902141</v>
+        <v>0.9287414022295643</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.3126622125947304</v>
+        <v>0.9204364628324617</v>
       </c>
       <c r="C8" t="n">
-        <v>0.09373976290225983</v>
+        <v>0.8226803541183472</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4064019754969903</v>
+        <v>0.09775610871411455</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7110342685963754</v>
+        <v>0.9109491553377701</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.5370153890333127</v>
+        <v>0.1157081154807911</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.1019731312990189</v>
+        <v>0.214569479227066</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4350422577342938</v>
+        <v>0.09886136374627495</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6968435909189481</v>
+        <v>0.9100329058715528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added model training and feature results
</commit_message>
<xml_diff>
--- a/Results/Breguets_Range/CNN_Confidence_score.xlsx
+++ b/Results/Breguets_Range/CNN_Confidence_score.xlsx
@@ -457,138 +457,138 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1839054330529666</v>
+        <v>0.2590361445783131</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2158649861812592</v>
+        <v>0.2453109174966812</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03195955312829257</v>
+        <v>0.01372522708163193</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9690302269779759</v>
+        <v>0.9864606042002675</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3009774948852012</v>
+        <v>0.2048192771084338</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2567024827003479</v>
+        <v>0.2393135130405426</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0442750121848533</v>
+        <v>0.03449423593210885</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9576021530073574</v>
+        <v>0.9666559418757626</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0.106615139804501</v>
+        <v>0.1927710843373494</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1699984669685364</v>
+        <v>0.2334723174571991</v>
       </c>
       <c r="D4" t="n">
-        <v>0.06338332716403534</v>
+        <v>0.04070123311984972</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9403946577448473</v>
+        <v>0.9608905689504814</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.09297567629006591</v>
+        <v>0.9156626506024095</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1655720621347427</v>
+        <v>0.9610681533813477</v>
       </c>
       <c r="D5" t="n">
-        <v>0.07259638584467683</v>
+        <v>0.04540550277893818</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9323171448246987</v>
+        <v>0.9565666120388313</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.238463287110707</v>
+        <v>0.06265060240963854</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3150076270103455</v>
+        <v>0.1267924308776855</v>
       </c>
       <c r="D6" t="n">
-        <v>0.07654433989963849</v>
+        <v>0.064141828468047</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9288981075254418</v>
+        <v>0.9397243612156601</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2498295067060696</v>
+        <v>0.1349397590361446</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3265554904937744</v>
+        <v>0.2219508737325668</v>
       </c>
       <c r="D7" t="n">
-        <v>0.07672598378770479</v>
+        <v>0.08701111469642228</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9287414022295643</v>
+        <v>0.9199537948416263</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9204364628324617</v>
+        <v>0.03855421686746985</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8226803541183472</v>
+        <v>0.1274387687444687</v>
       </c>
       <c r="D8" t="n">
-        <v>0.09775610871411455</v>
+        <v>0.08888455187699884</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9109491553377701</v>
+        <v>0.918371004783031</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1157081154807911</v>
+        <v>0.05301204819277108</v>
       </c>
       <c r="C9" t="n">
-        <v>0.214569479227066</v>
+        <v>0.1701029539108276</v>
       </c>
       <c r="D9" t="n">
-        <v>0.09886136374627495</v>
+        <v>0.1170909057180566</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9100329058715528</v>
+        <v>0.8951822943695066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>